<commit_message>
update cost/* to v1.1
Signed-off-by: socrates77 <zhwenrong@sina.com>
</commit_message>
<xml_diff>
--- a/cost/summary_200413.xlsx
+++ b/cost/summary_200413.xlsx
@@ -6,7 +6,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4月" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4月-大类" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4月-项目" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -57,7 +58,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -69,6 +70,50 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -91,17 +136,19 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="6" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -476,4 +523,307 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>通用和遥控器</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>锂电数码</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>家用电器</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n"/>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>A890</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>A880</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>A870</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>A811</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>A840</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>A860</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>A830</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>A680</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>A720</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>A780</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>A801</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>A800</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>A820</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>A700</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="inlineStr">
+        <is>
+          <t>A730</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="inlineStr">
+        <is>
+          <t>A740</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>基本工资</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>809.25</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>4681.02</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>974.9500000000002</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>791.33</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>974.9500000000002</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>687.9000000000001</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>343.95</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>343.95</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>137.58</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>1844.23</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>8747.900000000001</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>318.08</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>819.8500000000001</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>687.9000000000001</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>137.58</v>
+      </c>
+      <c r="Q3" s="3" t="n">
+        <v>137.58</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>岗位工资</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>2719</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>12144.98</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>2044.9</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>1705.52</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>2044.9</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>1583.6</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>791.8</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>791.8</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>316.72</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>4759.42</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>22015.1</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>903.72</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>1402.5</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <v>1583.6</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>316.72</v>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>316.72</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>补贴</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>221.85</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>1072.8</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>181.45</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>166.35</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>181.45</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>60.75</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>60.75</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>400.75</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>2232</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>99.2</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>127.75</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="Q5" s="3" t="n">
+        <v>24.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:Q1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>